<commit_message>
first draft unit tests; refactored for robustness and compartamentalization
</commit_message>
<xml_diff>
--- a/unit_tests.xlsx
+++ b/unit_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clemo\git\gesture_recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19B5E621-DC31-4565-9AC4-999610689960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0ABF77-A238-4765-8C05-0458E4D09515}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B642C369-E3B7-449B-90D3-11B977FBF9DF}"/>
   </bookViews>
@@ -35,32 +35,130 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>setup</t>
   </si>
   <si>
-    <t>teardown</t>
-  </si>
-  <si>
-    <t>get_headers</t>
-  </si>
-  <si>
-    <t>post</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
-    <t>put</t>
+    <t>disconnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">improperly sized frame processed </t>
+  </si>
+  <si>
+    <t>properly sized frame processed</t>
+  </si>
+  <si>
+    <t>Featurizer - process</t>
+  </si>
+  <si>
+    <t>predictor</t>
+  </si>
+  <si>
+    <t>assert output dimensions</t>
+  </si>
+  <si>
+    <t>assert binary image output</t>
+  </si>
+  <si>
+    <t>api/tokens</t>
+  </si>
+  <si>
+    <t>api/users</t>
+  </si>
+  <si>
+    <t>blank or no username or password - return 401</t>
+  </si>
+  <si>
+    <t>incorrect password - return 401</t>
+  </si>
+  <si>
+    <t>successful authentication - return 200, token</t>
+  </si>
+  <si>
+    <t>get user list - return 200, dictionary with 'users' where each user dictionary includes only 'online' and 'username'</t>
+  </si>
+  <si>
+    <t>blank or no username or password - return 400</t>
+  </si>
+  <si>
+    <t>register duplicate user - return 400</t>
+  </si>
+  <si>
+    <t>successful registration - return 200, token</t>
+  </si>
+  <si>
+    <t>socketio</t>
+  </si>
+  <si>
+    <t>setup application</t>
+  </si>
+  <si>
+    <t>teardown application</t>
+  </si>
+  <si>
+    <t>configure POST API compatibility</t>
+  </si>
+  <si>
+    <t>configure GET API compatibility</t>
+  </si>
+  <si>
+    <t>configure request header compatibility</t>
+  </si>
+  <si>
+    <t>improper image depth (should be 3)</t>
+  </si>
+  <si>
+    <t>improper command (not r or b)</t>
+  </si>
+  <si>
+    <t>missing data</t>
+  </si>
+  <si>
+    <t>improper image datatype</t>
+  </si>
+  <si>
+    <t>improper image shape (should be 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">token does not belong to user </t>
+  </si>
+  <si>
+    <t>incomplete data (missing image, token, command, or gesture)</t>
+  </si>
+  <si>
+    <t>featurizer</t>
+  </si>
+  <si>
+    <t>verify that image has shape 144x256 when exiting process()</t>
+  </si>
+  <si>
+    <t>frame shape not equal to current background frame shape</t>
+  </si>
+  <si>
+    <t>improper gesture (not in gesture_map) - check outputs label, pred_Gest, pred_conf, time</t>
+  </si>
+  <si>
+    <t>no prediction of session['pause_count'] &lt; 2</t>
+  </si>
+  <si>
+    <t>press 'b' if start_countdown false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -88,8 +186,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,54 +503,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD460DF3-965D-44EB-9A43-EAC50C7735FA}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>